<commit_message>
Actualizacion final estructura de evidencia github
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencias de documentación/Sprint Planning  - Proyecto Biblioteca El pimiento.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencias de documentación/Sprint Planning  - Proyecto Biblioteca El pimiento.xlsx
@@ -140,19 +140,19 @@
     <t>Crud funciones secundarias</t>
   </si>
   <si>
+    <t>Pagina principal administradores</t>
+  </si>
+  <si>
     <t>Filtro</t>
   </si>
   <si>
-    <t>Pagina principal administradores</t>
-  </si>
-  <si>
     <t>Seguridad pagina</t>
   </si>
   <si>
     <t>Pagina principal usuarios</t>
   </si>
   <si>
-    <t>Pagina informativa</t>
+    <t>Pagina principal informativa</t>
   </si>
   <si>
     <t>Poblado de base de datos</t>
@@ -167,7 +167,7 @@
     <t>adaptabilidad a celulares</t>
   </si>
   <si>
-    <t>No empezado</t>
+    <t>Cancelado</t>
   </si>
   <si>
     <t>Marcha blanca</t>
@@ -799,11 +799,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1615589012"/>
-        <c:axId val="867146787"/>
+        <c:axId val="514574586"/>
+        <c:axId val="414836133"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1615589012"/>
+        <c:axId val="514574586"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,10 +855,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867146787"/>
+        <c:crossAx val="414836133"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867146787"/>
+        <c:axId val="414836133"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +933,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1615589012"/>
+        <c:crossAx val="514574586"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1120,11 +1120,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1878405385"/>
-        <c:axId val="1165184134"/>
+        <c:axId val="1919263294"/>
+        <c:axId val="452862767"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1878405385"/>
+        <c:axId val="1919263294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1176,10 +1176,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1165184134"/>
+        <c:crossAx val="452862767"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1165184134"/>
+        <c:axId val="452862767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1254,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1878405385"/>
+        <c:crossAx val="1919263294"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1418,11 +1418,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1645091540"/>
-        <c:axId val="1974959301"/>
+        <c:axId val="513646899"/>
+        <c:axId val="314753752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1645091540"/>
+        <c:axId val="513646899"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,10 +1474,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1974959301"/>
+        <c:crossAx val="314753752"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1974959301"/>
+        <c:axId val="314753752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1552,7 +1552,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1645091540"/>
+        <c:crossAx val="513646899"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1728,11 +1728,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1121083009"/>
-        <c:axId val="48973305"/>
+        <c:axId val="536236549"/>
+        <c:axId val="2077747975"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1121083009"/>
+        <c:axId val="536236549"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,10 +1784,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48973305"/>
+        <c:crossAx val="2077747975"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48973305"/>
+        <c:axId val="2077747975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1862,7 +1862,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1121083009"/>
+        <c:crossAx val="536236549"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2311,10 +2311,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="17">
-        <v>45564.0</v>
+        <v>45551.0</v>
       </c>
       <c r="F6" s="17">
-        <v>45564.0</v>
+        <v>45551.0</v>
       </c>
       <c r="G6" s="18">
         <v>1.0</v>
@@ -2335,10 +2335,10 @@
         <v>11</v>
       </c>
       <c r="E7" s="23">
-        <v>45564.0</v>
+        <v>45552.0</v>
       </c>
       <c r="F7" s="23">
-        <v>45564.0</v>
+        <v>45554.0</v>
       </c>
       <c r="G7" s="24">
         <v>3.0</v>
@@ -2359,10 +2359,10 @@
         <v>11</v>
       </c>
       <c r="E8" s="17">
-        <v>45564.0</v>
+        <v>45555.0</v>
       </c>
       <c r="F8" s="17">
-        <v>45564.0</v>
+        <v>45556.0</v>
       </c>
       <c r="G8" s="18">
         <v>2.0</v>
@@ -2383,10 +2383,10 @@
         <v>11</v>
       </c>
       <c r="E9" s="23">
-        <v>45563.0</v>
+        <v>45558.0</v>
       </c>
       <c r="F9" s="23">
-        <v>45563.0</v>
+        <v>45560.0</v>
       </c>
       <c r="G9" s="24">
         <v>2.0</v>
@@ -2407,10 +2407,10 @@
         <v>11</v>
       </c>
       <c r="E10" s="17">
-        <v>45564.0</v>
+        <v>45561.0</v>
       </c>
       <c r="F10" s="17">
-        <v>45564.0</v>
+        <v>45562.0</v>
       </c>
       <c r="G10" s="18">
         <v>4.0</v>
@@ -2887,7 +2887,7 @@
         <v>11</v>
       </c>
       <c r="E31" s="31">
-        <v>45600.0</v>
+        <v>45593.0</v>
       </c>
       <c r="F31" s="31">
         <v>45604.0</v>
@@ -2904,31 +2904,31 @@
     </row>
     <row r="32">
       <c r="B32" s="14"/>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="28" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="32">
-        <v>45600.0</v>
+        <v>45597.0</v>
       </c>
       <c r="F32" s="32">
-        <v>45603.0</v>
+        <v>45601.0</v>
       </c>
       <c r="G32" s="18">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="H32" s="18">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="20"/>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="30" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="22" t="s">
@@ -2938,16 +2938,16 @@
         <v>45600.0</v>
       </c>
       <c r="F33" s="31">
-        <v>45601.0</v>
+        <v>45603.0</v>
       </c>
       <c r="G33" s="24">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="H33" s="24">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="I33" s="25" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34">
@@ -3040,7 +3040,7 @@
         <v>12.0</v>
       </c>
       <c r="H37" s="24">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="I37" s="25" t="s">
         <v>12</v>
@@ -3112,7 +3112,7 @@
         <v>51</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E41" s="31">
         <v>45621.0</v>
@@ -3124,7 +3124,7 @@
         <v>10.0</v>
       </c>
       <c r="H41" s="24">
-        <v>0.0</v>
+        <v>37.0</v>
       </c>
       <c r="I41" s="25" t="s">
         <v>12</v>
@@ -3136,7 +3136,7 @@
         <v>52</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E42" s="32">
         <v>45621.0</v>
@@ -3148,7 +3148,7 @@
         <v>10.0</v>
       </c>
       <c r="H42" s="18">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="I42" s="19" t="s">
         <v>12</v>
@@ -3160,7 +3160,7 @@
         <v>53</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E43" s="31">
         <v>45621.0</v>
@@ -3172,7 +3172,7 @@
         <v>10.0</v>
       </c>
       <c r="H43" s="24">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="I43" s="25" t="s">
         <v>12</v>
@@ -3192,14 +3192,14 @@
       </c>
       <c r="H44" s="38">
         <f t="shared" si="1"/>
-        <v>176</v>
+        <v>227</v>
       </c>
       <c r="I44" s="39"/>
     </row>
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" sqref="D5:D44">
-      <formula1>"Terminado,Desarrollo,No empezado,Atrasado"</formula1>
+      <formula1>"Terminado,Desarrollo,No empezado,Atrasado,Cancelado"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="I5:I44">
       <formula1>"Scrum master,Scrum team,Sebastian Gonzalez,Sebastian Pardo,Sin asignar"</formula1>

</xml_diff>